<commit_message>
new fixes description of the first page
</commit_message>
<xml_diff>
--- a/src/data/inputData/input.xlsx
+++ b/src/data/inputData/input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\makuznetsova\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\makuznetsova\Documents\sample\src\data\inputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,13 +26,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Снять</t>
+    <t>Воронеж</t>
   </si>
   <si>
-    <t>Квартиру</t>
+    <t>Купить</t>
   </si>
   <si>
-    <t>Воронеж</t>
+    <t>Комната</t>
   </si>
 </sst>
 </file>
@@ -351,35 +351,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="5" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>1000</v>
+      </c>
+      <c r="D1">
+        <v>1000000000</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>10000</v>
-      </c>
-      <c r="E1">
-        <v>30000</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>